<commit_message>
Finished simulation portion of report
</commit_message>
<xml_diff>
--- a/Circuit Design/Analysis/Data Comparison.xlsx
+++ b/Circuit Design/Analysis/Data Comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zelli\Documents\Personal Projects\Electronics\TRIAC-Dimmer\Circuit Design\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2952D1AC-B0AE-46BA-9536-9D1E2E72A686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BB8EA0-738E-4F32-AB2B-7FDABE5085FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0k" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="18">
   <si>
     <t>Simulation</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Peak 3</t>
+  </si>
+  <si>
+    <t>Breakover</t>
   </si>
 </sst>
 </file>
@@ -95,7 +98,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -128,10 +131,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -604,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAB08283-946F-4EFB-89F2-F6DB5B61551A}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,14 +814,237 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA1E142-24AB-422F-8192-17B9C58EC691}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1">
+        <v>5.8900000000000003E-3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>135.36702102541784</v>
+      </c>
+      <c r="D3" s="1">
+        <v>32.018483442221992</v>
+      </c>
+      <c r="E3" s="1">
+        <v>5.9319608101839998E-3</v>
+      </c>
+      <c r="F3" s="1">
+        <v>133.72336431279999</v>
+      </c>
+      <c r="G3" s="1">
+        <v>32.108808872269996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.6209999999999999E-2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>28.912224463505513</v>
+      </c>
+      <c r="D4" s="1">
+        <v>28.54618047946137</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1.6253811708870001E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>26.3525525907</v>
+      </c>
+      <c r="G4" s="1">
+        <v>28.397575403689999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3.2939999999999997E-2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>24.904558197196039</v>
+      </c>
+      <c r="D5" s="1">
+        <v>24.958450651225178</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3.2972625278340002E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>23.046054784300001</v>
+      </c>
+      <c r="G5" s="1">
+        <v>24.82900158544</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4.9630000000000001E-2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>23.424349416388619</v>
+      </c>
+      <c r="D6" s="1">
+        <v>23.391896131682675</v>
+      </c>
+      <c r="E6" s="1">
+        <v>4.9668035387330001E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <v>21.219619325099998</v>
+      </c>
+      <c r="G6" s="1">
+        <v>23.282985685100002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1">
+        <v>6.6309999999999994E-2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>22.577694694958705</v>
+      </c>
+      <c r="D7" s="1">
+        <v>22.707096657410428</v>
+      </c>
+      <c r="E7" s="1">
+        <v>6.6281809973049999E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>24.578441169569999</v>
+      </c>
+      <c r="G7" s="1">
+        <v>22.613559857119998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1">
+        <v>8.2979999999999998E-2</v>
+      </c>
+      <c r="C8" s="1">
+        <v>22.365941045689226</v>
+      </c>
+      <c r="D8" s="1">
+        <v>22.407608274481422</v>
+      </c>
+      <c r="E8" s="1">
+        <v>8.2991990370249999E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>21.81582915381</v>
+      </c>
+      <c r="G8" s="1">
+        <v>22.32547890283</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1">
+        <v>9.9650000000000002E-2</v>
+      </c>
+      <c r="C9" s="1">
+        <v>22.154152077545362</v>
+      </c>
+      <c r="D9" s="1">
+        <v>22.276591015932237</v>
+      </c>
+      <c r="E9" s="1">
+        <v>9.9675309735200002E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <v>20.756984194880001</v>
+      </c>
+      <c r="G9" s="1">
+        <v>22.1987763395</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>